<commit_message>
jobs module: added subpackage for results
</commit_message>
<xml_diff>
--- a/emx/dist/jobs.xlsx
+++ b/emx/dist/jobs.xlsx
@@ -17,17 +17,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>jobs</t>
   </si>
   <si>
+    <t>jobs_results</t>
+  </si>
+  <si>
     <t>Jobs</t>
   </si>
   <si>
+    <t>Results</t>
+  </si>
+  <si>
     <t>Overview and statuses of custom processes run in this database (v0.9.0, 2021-10-28)</t>
   </si>
   <si>
+    <t>The outcome of process including analyzed data.</t>
+  </si>
+  <si>
     <t>processStatus</t>
   </si>
   <si>
@@ -140,6 +149,9 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>parent</t>
   </si>
   <si>
     <t>package</t>
@@ -610,32 +622,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -653,16 +682,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -673,10 +702,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -684,13 +713,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -708,39 +737,39 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -749,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -760,10 +789,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -772,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -781,15 +810,15 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -798,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -807,15 +836,15 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -824,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -833,15 +862,15 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -850,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -859,15 +888,15 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -876,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -885,15 +914,15 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -902,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -911,18 +940,18 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -931,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -940,15 +969,15 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -957,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -966,15 +995,15 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -983,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -992,15 +1021,15 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -1009,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1018,15 +1047,15 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1035,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1044,15 +1073,15 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1061,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1070,15 +1099,15 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1087,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1096,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1114,138 +1143,138 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>